<commit_message>
add row to hit-miss table for chocie rule & text editing
</commit_message>
<xml_diff>
--- a/Tables/hit_miss_rule.xlsx
+++ b/Tables/hit_miss_rule.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D2008A-A0D2-436D-A1AE-2F69B7FE4995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DC6D42-844E-4B7C-A6CB-98B968658DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500"/>
+    <workbookView xWindow="-24525" yWindow="2565" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hit_miss_rule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Rule</t>
   </si>
@@ -50,18 +50,12 @@
     <t>Optimal</t>
   </si>
   <si>
-    <t>% incorrectly assing to treatment</t>
-  </si>
-  <si>
     <t>Narrow rule (RF)</t>
   </si>
   <si>
     <t>Narrow rule (Logit)</t>
   </si>
   <si>
-    <t xml:space="preserve">% incorrectly assing to control </t>
-  </si>
-  <si>
     <t>(Type I)</t>
   </si>
   <si>
@@ -75,13 +69,22 @@
   </si>
   <si>
     <t>T2</t>
+  </si>
+  <si>
+    <t>Choice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% incorrectly assigned to control </t>
+  </si>
+  <si>
+    <t>% incorrectly assigned to treatment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,19 +133,19 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -163,7 +166,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -314,7 +317,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -338,9 +341,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -364,7 +367,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -399,7 +402,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -417,7 +420,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -442,7 +445,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -458,58 +461,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6318840B-C0A0-47C6-A36C-67296A34F7B3}">
-  <dimension ref="C3:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6318840B-C0A0-47C6-A36C-67296A34F7B3}">
+  <dimension ref="C3:J11"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.54296875" style="5" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="26.54296875" style="1" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="29.26953125" style="1" bestFit="true" customWidth="true"/>
-    <col min="6" max="6" width="13.36328125" style="1" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="4"/>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" ht="15" thickTop="true" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1">
         <f>ROUND(H5,2)</f>
-        <v>91</v>
+        <v>86.65</v>
       </c>
       <c r="E5" s="1">
         <f>ROUND(I5,2)</f>
@@ -517,13 +520,13 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" ref="F5:F8" si="0">SUM(D5:E5)</f>
-        <v>91</v>
+        <v>86.65</v>
       </c>
       <c r="H5">
-        <v>86.65456390380859</v>
-      </c>
-    </row>
-    <row r="6" x14ac:dyDescent="0.35">
+        <v>86.654563903808594</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
@@ -533,17 +536,17 @@
       </c>
       <c r="E6" s="1">
         <f t="shared" ref="E6:E9" si="2">ROUND(I6,2)</f>
-        <v>9</v>
+        <v>13.35</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>13.35</v>
       </c>
       <c r="I6" s="1">
         <v>13.34543609619141</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
         <v>3</v>
       </c>
@@ -560,53 +563,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="1"/>
-        <v>0.48</v>
+        <v>5.42</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="2"/>
-        <v>7.13</v>
+        <v>6.25</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>7.6099999999999994</v>
+        <v>11.67</v>
       </c>
       <c r="H8">
-        <v>5.415094375610352</v>
+        <v>5.4150943756103516</v>
       </c>
       <c r="I8">
-        <v>6.245283126831055</v>
-      </c>
-    </row>
-    <row r="9" ht="15" thickBot="true" x14ac:dyDescent="0.4">
-      <c r="C9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2">
+        <v>6.2452831268310547</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1">
         <f t="shared" si="1"/>
-        <v>7.68</v>
-      </c>
-      <c r="E9" s="2">
+        <v>9.36</v>
+      </c>
+      <c r="E9" s="1">
         <f t="shared" si="2"/>
-        <v>7.33</v>
-      </c>
-      <c r="F9" s="2">
+        <v>10.24</v>
+      </c>
+      <c r="F9" s="1">
         <f>SUM(D9:E9)</f>
-        <v>15.01</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="H9">
-        <v>9.362844467163086</v>
+        <v>9.3628444671630859</v>
       </c>
       <c r="I9">
-        <v>10.24238014221191</v>
-      </c>
-    </row>
-    <row r="10" ht="15" thickTop="true" x14ac:dyDescent="0.35"/>
+        <v>10.242380142211911</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" ref="D10" si="3">ROUND(H10,2)</f>
+        <v>80.3</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" ref="E10" si="4">ROUND(I10,2)</f>
+        <v>21.37</v>
+      </c>
+      <c r="F10" s="2">
+        <f>ROUND(J10,2)</f>
+        <v>71.23</v>
+      </c>
+      <c r="H10">
+        <v>80.296737670898438</v>
+      </c>
+      <c r="I10">
+        <v>21.367921829223629</v>
+      </c>
+      <c r="J10">
+        <v>71.23077392578125</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add loan as predictor in narrow and wide forest
</commit_message>
<xml_diff>
--- a/Tables/hit_miss_rule.xlsx
+++ b/Tables/hit_miss_rule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DC6D42-844E-4B7C-A6CB-98B968658DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581F58B9-DD39-40DD-BE41-445051A92E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24525" yWindow="2565" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24360" yWindow="2370" windowWidth="21585" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hit_miss_rule" sheetId="1" r:id="rId1"/>
@@ -512,7 +512,7 @@
       </c>
       <c r="D5" s="1">
         <f>ROUND(H5,2)</f>
-        <v>86.65</v>
+        <v>91.22</v>
       </c>
       <c r="E5" s="1">
         <f>ROUND(I5,2)</f>
@@ -520,10 +520,10 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" ref="F5:F8" si="0">SUM(D5:E5)</f>
-        <v>86.65</v>
+        <v>91.22</v>
       </c>
       <c r="H5">
-        <v>86.654563903808594</v>
+        <v>91.224967956542969</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
@@ -536,14 +536,14 @@
       </c>
       <c r="E6" s="1">
         <f t="shared" ref="E6:E9" si="2">ROUND(I6,2)</f>
-        <v>13.35</v>
+        <v>8.7799999999999994</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>13.35</v>
+        <v>8.7799999999999994</v>
       </c>
       <c r="I6" s="1">
-        <v>13.34543609619141</v>
+        <v>8.7750320434570313</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
@@ -569,21 +569,21 @@
       </c>
       <c r="D8" s="1">
         <f t="shared" si="1"/>
-        <v>5.42</v>
+        <v>3.72</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="2"/>
-        <v>6.25</v>
+        <v>4.55</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>11.67</v>
+        <v>8.27</v>
       </c>
       <c r="H8">
-        <v>5.4150943756103516</v>
+        <v>3.7213354110717769</v>
       </c>
       <c r="I8">
-        <v>6.2452831268310547</v>
+        <v>4.5544266700744629</v>
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
@@ -592,21 +592,21 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="1"/>
-        <v>9.36</v>
+        <v>6.6</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="2"/>
-        <v>10.24</v>
+        <v>7.44</v>
       </c>
       <c r="F9" s="1">
         <f>SUM(D9:E9)</f>
-        <v>19.600000000000001</v>
+        <v>14.04</v>
       </c>
       <c r="H9">
-        <v>9.3628444671630859</v>
+        <v>6.5950651168823242</v>
       </c>
       <c r="I9">
-        <v>10.242380142211911</v>
+        <v>7.4397678375244141</v>
       </c>
     </row>
     <row r="10" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -615,24 +615,24 @@
       </c>
       <c r="D10" s="2">
         <f t="shared" ref="D10" si="3">ROUND(H10,2)</f>
-        <v>80.3</v>
+        <v>77.02</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" ref="E10" si="4">ROUND(I10,2)</f>
-        <v>21.37</v>
+        <v>17.84</v>
       </c>
       <c r="F10" s="2">
         <f>ROUND(J10,2)</f>
-        <v>71.23</v>
+        <v>67.91</v>
       </c>
       <c r="H10">
-        <v>80.296737670898438</v>
+        <v>77.015411376953125</v>
       </c>
       <c r="I10">
-        <v>21.367921829223629</v>
+        <v>17.839620590209961</v>
       </c>
       <c r="J10">
-        <v>71.23077392578125</v>
+        <v>67.911468505859375</v>
       </c>
     </row>
     <row r="11" spans="3:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>